<commit_message>
Update vai cai task moi ccho ngay mai
</commit_message>
<xml_diff>
--- a/Documents/Task Sheet/TaskSheet.xlsx
+++ b/Documents/Task Sheet/TaskSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="191">
   <si>
     <t>No.</t>
   </si>
@@ -938,6 +938,28 @@
   </si>
   <si>
     <t>07/06/2015</t>
+  </si>
+  <si>
+    <t>study AJAX</t>
+  </si>
+  <si>
+    <t>study Notification</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">study how to create forum, upload download </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>files</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1007,7 +1029,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1080,6 +1102,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1108,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1190,9 +1218,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1238,6 +1263,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1542,21 +1573,21 @@
   <dimension ref="A1:S173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" style="13" customWidth="1"/>
     <col min="13" max="13" width="6.140625" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" style="13" customWidth="1"/>
-    <col min="16" max="16" width="16" style="31" customWidth="1"/>
-    <col min="17" max="17" width="11" style="31" customWidth="1"/>
+    <col min="16" max="16" width="16" style="30" customWidth="1"/>
+    <col min="17" max="17" width="11" style="30" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1594,12 +1625,12 @@
       <c r="K1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44" t="s">
+      <c r="M1" s="42"/>
+      <c r="N1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="45"/>
-      <c r="P1" s="40" t="s">
+      <c r="O1" s="44"/>
+      <c r="P1" s="39" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1629,16 +1660,16 @@
       <c r="I2" s="3"/>
       <c r="J2" s="1"/>
       <c r="K2" s="12"/>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="47" t="s">
+      <c r="N2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="39" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1668,22 +1699,22 @@
       <c r="I3" s="3"/>
       <c r="J3" s="1"/>
       <c r="K3" s="12"/>
-      <c r="M3" s="30">
+      <c r="M3" s="29">
         <v>1</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="N3" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="O3" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P3" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="R3" s="42" t="s">
+      <c r="R3" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="S3" s="33" t="s">
         <v>183</v>
       </c>
     </row>
@@ -1713,22 +1744,22 @@
       <c r="I4" s="3"/>
       <c r="J4" s="1"/>
       <c r="K4" s="12"/>
-      <c r="M4" s="30">
+      <c r="M4" s="29">
         <v>2</v>
       </c>
-      <c r="N4" s="32" t="s">
+      <c r="N4" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P4" s="33" t="s">
+      <c r="P4" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="R4" s="42" t="s">
+      <c r="R4" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="S4" s="34" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1758,22 +1789,22 @@
       <c r="I5" s="3"/>
       <c r="J5" s="1"/>
       <c r="K5" s="12"/>
-      <c r="M5" s="30">
+      <c r="M5" s="29">
         <v>3</v>
       </c>
-      <c r="N5" s="32" t="s">
+      <c r="N5" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="O5" s="34" t="s">
+      <c r="O5" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P5" s="33" t="s">
+      <c r="P5" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="R5" s="42" t="s">
+      <c r="R5" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="S5" s="36" t="s">
+      <c r="S5" s="35" t="s">
         <v>184</v>
       </c>
     </row>
@@ -1799,22 +1830,22 @@
         <v>18</v>
       </c>
       <c r="K6" s="12"/>
-      <c r="M6" s="30">
+      <c r="M6" s="29">
         <v>4</v>
       </c>
-      <c r="N6" s="32" t="s">
+      <c r="N6" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="O6" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="P6" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="R6" s="42" t="s">
+      <c r="R6" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="S6" s="37" t="s">
+      <c r="S6" s="36" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1840,16 +1871,16 @@
         <v>18</v>
       </c>
       <c r="K7" s="12"/>
-      <c r="M7" s="30">
+      <c r="M7" s="29">
         <v>5</v>
       </c>
-      <c r="N7" s="32" t="s">
+      <c r="N7" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="O7" s="34" t="s">
+      <c r="O7" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P7" s="33" t="s">
+      <c r="P7" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1873,16 +1904,16 @@
       <c r="K8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="29">
         <v>6</v>
       </c>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P8" s="33" t="s">
+      <c r="P8" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1908,16 +1939,16 @@
         <v>32</v>
       </c>
       <c r="K9" s="12"/>
-      <c r="M9" s="30">
+      <c r="M9" s="29">
         <v>7</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="O9" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P9" s="33" t="s">
+      <c r="P9" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1943,19 +1974,19 @@
         <v>32</v>
       </c>
       <c r="K10" s="12"/>
-      <c r="M10" s="30">
+      <c r="M10" s="29">
         <v>8</v>
       </c>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="O10" s="34" t="s">
+      <c r="O10" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P10" s="33" t="s">
+      <c r="P10" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="Q10" s="41"/>
+      <c r="Q10" s="40"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="2">
@@ -1979,16 +2010,16 @@
         <v>31</v>
       </c>
       <c r="K11" s="12"/>
-      <c r="M11" s="30">
+      <c r="M11" s="29">
         <v>9</v>
       </c>
-      <c r="N11" s="32" t="s">
+      <c r="N11" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="O11" s="34" t="s">
+      <c r="O11" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P11" s="33" t="s">
+      <c r="P11" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2014,16 +2045,16 @@
         <v>3</v>
       </c>
       <c r="K12" s="12"/>
-      <c r="M12" s="30">
+      <c r="M12" s="29">
         <v>10</v>
       </c>
-      <c r="N12" s="32" t="s">
+      <c r="N12" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P12" s="33" t="s">
+      <c r="P12" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2045,16 +2076,16 @@
       <c r="I13" s="3"/>
       <c r="J13" s="1"/>
       <c r="K13" s="12"/>
-      <c r="M13" s="30">
-        <v>11</v>
-      </c>
-      <c r="N13" s="32" t="s">
+      <c r="M13" s="29">
+        <v>11</v>
+      </c>
+      <c r="N13" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="O13" s="37" t="s">
+      <c r="O13" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P13" s="33" t="s">
+      <c r="P13" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2082,16 +2113,16 @@
         <v>5</v>
       </c>
       <c r="K14" s="12"/>
-      <c r="M14" s="30">
+      <c r="M14" s="29">
         <v>12</v>
       </c>
-      <c r="N14" s="32" t="s">
+      <c r="N14" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="O14" s="36" t="s">
+      <c r="O14" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P14" s="33" t="s">
+      <c r="P14" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2117,16 +2148,16 @@
         <v>3</v>
       </c>
       <c r="K15" s="12"/>
-      <c r="M15" s="30">
+      <c r="M15" s="29">
         <v>13</v>
       </c>
-      <c r="N15" s="32" t="s">
+      <c r="N15" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="O15" s="36" t="s">
+      <c r="O15" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P15" s="33" t="s">
+      <c r="P15" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2152,16 +2183,16 @@
         <v>3</v>
       </c>
       <c r="K16" s="12"/>
-      <c r="M16" s="30">
+      <c r="M16" s="29">
         <v>14</v>
       </c>
-      <c r="N16" s="32" t="s">
+      <c r="N16" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="O16" s="36" t="s">
+      <c r="O16" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P16" s="33" t="s">
+      <c r="P16" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2187,16 +2218,16 @@
       <c r="K17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="M17" s="30">
+      <c r="M17" s="29">
         <v>15</v>
       </c>
-      <c r="N17" s="32" t="s">
+      <c r="N17" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P17" s="33" t="s">
+      <c r="P17" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2222,16 +2253,16 @@
         <v>3</v>
       </c>
       <c r="K18" s="12"/>
-      <c r="M18" s="30">
+      <c r="M18" s="29">
         <v>16</v>
       </c>
-      <c r="N18" s="32" t="s">
+      <c r="N18" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="O18" s="35" t="s">
+      <c r="O18" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P18" s="33" t="s">
+      <c r="P18" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2257,16 +2288,16 @@
       <c r="K19" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="30">
+      <c r="M19" s="29">
         <v>17</v>
       </c>
-      <c r="N19" s="32" t="s">
+      <c r="N19" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="O19" s="35" t="s">
+      <c r="O19" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P19" s="33" t="s">
+      <c r="P19" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2290,16 +2321,16 @@
       <c r="I20" s="3"/>
       <c r="J20" s="1"/>
       <c r="K20" s="12"/>
-      <c r="M20" s="30">
+      <c r="M20" s="29">
         <v>18</v>
       </c>
-      <c r="N20" s="32" t="s">
+      <c r="N20" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="O20" s="37" t="s">
+      <c r="O20" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P20" s="33" t="s">
+      <c r="P20" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2323,16 +2354,16 @@
       <c r="I21" s="3"/>
       <c r="J21" s="1"/>
       <c r="K21" s="12"/>
-      <c r="M21" s="30">
+      <c r="M21" s="29">
         <v>19</v>
       </c>
-      <c r="N21" s="32" t="s">
+      <c r="N21" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="O21" s="37" t="s">
+      <c r="O21" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P21" s="33" t="s">
+      <c r="P21" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2354,16 +2385,16 @@
       <c r="I22" s="3"/>
       <c r="J22" s="1"/>
       <c r="K22" s="12"/>
-      <c r="M22" s="30">
+      <c r="M22" s="29">
         <v>20</v>
       </c>
-      <c r="N22" s="32" t="s">
+      <c r="N22" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="O22" s="37" t="s">
+      <c r="O22" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P22" s="33" t="s">
+      <c r="P22" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2385,16 +2416,16 @@
       <c r="I23" s="3"/>
       <c r="J23" s="1"/>
       <c r="K23" s="12"/>
-      <c r="M23" s="30">
+      <c r="M23" s="29">
         <v>21</v>
       </c>
-      <c r="N23" s="32" t="s">
+      <c r="N23" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="O23" s="37" t="s">
+      <c r="O23" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P23" s="33" t="s">
+      <c r="P23" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2418,16 +2449,16 @@
       <c r="I24" s="3"/>
       <c r="J24" s="1"/>
       <c r="K24" s="12"/>
-      <c r="M24" s="30">
+      <c r="M24" s="29">
         <v>22</v>
       </c>
-      <c r="N24" s="32" t="s">
+      <c r="N24" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="O24" s="37" t="s">
+      <c r="O24" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P24" s="33" t="s">
+      <c r="P24" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2453,16 +2484,16 @@
         <v>3</v>
       </c>
       <c r="K25" s="12"/>
-      <c r="M25" s="30">
+      <c r="M25" s="29">
         <v>23</v>
       </c>
-      <c r="N25" s="32" t="s">
+      <c r="N25" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="O25" s="37" t="s">
+      <c r="O25" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P25" s="33" t="s">
+      <c r="P25" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2490,16 +2521,16 @@
         <v>4</v>
       </c>
       <c r="K26" s="12"/>
-      <c r="M26" s="30">
+      <c r="M26" s="29">
         <v>24</v>
       </c>
-      <c r="N26" s="32" t="s">
+      <c r="N26" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="O26" s="37" t="s">
+      <c r="O26" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P26" s="33" t="s">
+      <c r="P26" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2525,16 +2556,16 @@
         <v>46</v>
       </c>
       <c r="K27" s="12"/>
-      <c r="M27" s="30">
+      <c r="M27" s="29">
         <v>25</v>
       </c>
-      <c r="N27" s="32" t="s">
+      <c r="N27" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="O27" s="37" t="s">
+      <c r="O27" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P27" s="33" t="s">
+      <c r="P27" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2558,16 +2589,16 @@
       <c r="I28" s="3"/>
       <c r="J28" s="1"/>
       <c r="K28" s="12"/>
-      <c r="M28" s="30">
+      <c r="M28" s="29">
         <v>26</v>
       </c>
-      <c r="N28" s="32" t="s">
+      <c r="N28" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="O28" s="36" t="s">
+      <c r="O28" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P28" s="33" t="s">
+      <c r="P28" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2599,16 +2630,16 @@
         <v>31</v>
       </c>
       <c r="K29" s="12"/>
-      <c r="M29" s="30">
+      <c r="M29" s="29">
         <v>27</v>
       </c>
-      <c r="N29" s="32" t="s">
+      <c r="N29" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="O29" s="36" t="s">
+      <c r="O29" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P29" s="33" t="s">
+      <c r="P29" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2640,16 +2671,16 @@
         <v>31</v>
       </c>
       <c r="K30" s="12"/>
-      <c r="M30" s="30">
+      <c r="M30" s="29">
         <v>28</v>
       </c>
-      <c r="N30" s="32" t="s">
+      <c r="N30" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="O30" s="36" t="s">
+      <c r="O30" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P30" s="33" t="s">
+      <c r="P30" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2675,16 +2706,16 @@
         <v>3</v>
       </c>
       <c r="K31" s="12"/>
-      <c r="M31" s="30">
+      <c r="M31" s="29">
         <v>29</v>
       </c>
-      <c r="N31" s="32" t="s">
+      <c r="N31" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="O31" s="35" t="s">
+      <c r="O31" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P31" s="33" t="s">
+      <c r="P31" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2710,16 +2741,16 @@
         <v>5</v>
       </c>
       <c r="K32" s="12"/>
-      <c r="M32" s="30">
+      <c r="M32" s="29">
         <v>30</v>
       </c>
-      <c r="N32" s="32" t="s">
+      <c r="N32" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="O32" s="35" t="s">
+      <c r="O32" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P32" s="33" t="s">
+      <c r="P32" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2745,16 +2776,16 @@
         <v>3</v>
       </c>
       <c r="K33" s="12"/>
-      <c r="M33" s="30">
+      <c r="M33" s="29">
         <v>31</v>
       </c>
-      <c r="N33" s="32" t="s">
+      <c r="N33" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="O33" s="35" t="s">
+      <c r="O33" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P33" s="33" t="s">
+      <c r="P33" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2778,16 +2809,16 @@
       <c r="I34" s="3"/>
       <c r="J34" s="1"/>
       <c r="K34" s="12"/>
-      <c r="M34" s="30">
+      <c r="M34" s="29">
         <v>32</v>
       </c>
-      <c r="N34" s="32" t="s">
+      <c r="N34" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="O34" s="35" t="s">
+      <c r="O34" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P34" s="33" t="s">
+      <c r="P34" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2811,16 +2842,16 @@
       <c r="I35" s="3"/>
       <c r="J35" s="1"/>
       <c r="K35" s="12"/>
-      <c r="M35" s="30">
+      <c r="M35" s="29">
         <v>33</v>
       </c>
-      <c r="N35" s="32" t="s">
+      <c r="N35" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="O35" s="35" t="s">
+      <c r="O35" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P35" s="33" t="s">
+      <c r="P35" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2846,16 +2877,16 @@
       <c r="K36" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M36" s="30">
+      <c r="M36" s="29">
         <v>34</v>
       </c>
-      <c r="N36" s="32" t="s">
+      <c r="N36" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="O36" s="35" t="s">
+      <c r="O36" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P36" s="33" t="s">
+      <c r="P36" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2879,16 +2910,16 @@
       <c r="K37" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="M37" s="30">
+      <c r="M37" s="29">
         <v>35</v>
       </c>
-      <c r="N37" s="32" t="s">
+      <c r="N37" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O37" s="36" t="s">
+      <c r="O37" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P37" s="33" t="s">
+      <c r="P37" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2912,16 +2943,16 @@
       <c r="I38" s="3"/>
       <c r="J38" s="1"/>
       <c r="K38" s="12"/>
-      <c r="M38" s="30">
+      <c r="M38" s="29">
         <v>36</v>
       </c>
-      <c r="N38" s="32" t="s">
+      <c r="N38" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="O38" s="36" t="s">
+      <c r="O38" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P38" s="33" t="s">
+      <c r="P38" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2945,16 +2976,16 @@
       <c r="I39" s="3"/>
       <c r="J39" s="1"/>
       <c r="K39" s="12"/>
-      <c r="M39" s="30">
+      <c r="M39" s="29">
         <v>37</v>
       </c>
-      <c r="N39" s="32" t="s">
+      <c r="N39" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="O39" s="36" t="s">
+      <c r="O39" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P39" s="33" t="s">
+      <c r="P39" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2978,16 +3009,16 @@
       <c r="K40" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="M40" s="30">
+      <c r="M40" s="29">
         <v>38</v>
       </c>
-      <c r="N40" s="32" t="s">
+      <c r="N40" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="O40" s="34" t="s">
+      <c r="O40" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P40" s="33" t="s">
+      <c r="P40" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3011,16 +3042,16 @@
       <c r="K41" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="M41" s="30">
+      <c r="M41" s="29">
         <v>39</v>
       </c>
-      <c r="N41" s="32" t="s">
+      <c r="N41" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="O41" s="37" t="s">
+      <c r="O41" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P41" s="33" t="s">
+      <c r="P41" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3046,16 +3077,16 @@
       <c r="K42" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="M42" s="30">
+      <c r="M42" s="29">
         <v>40</v>
       </c>
-      <c r="N42" s="32" t="s">
+      <c r="N42" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="O42" s="35" t="s">
+      <c r="O42" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P42" s="33" t="s">
+      <c r="P42" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3083,16 +3114,16 @@
       <c r="K43" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="M43" s="30">
+      <c r="M43" s="29">
         <v>41</v>
       </c>
-      <c r="N43" s="32" t="s">
+      <c r="N43" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="O43" s="35" t="s">
+      <c r="O43" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P43" s="33" t="s">
+      <c r="P43" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3120,16 +3151,16 @@
       <c r="K44" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="M44" s="30">
+      <c r="M44" s="29">
         <v>42</v>
       </c>
-      <c r="N44" s="32" t="s">
+      <c r="N44" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="O44" s="35" t="s">
+      <c r="O44" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P44" s="33" t="s">
+      <c r="P44" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3157,16 +3188,16 @@
       <c r="K45" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="M45" s="30">
+      <c r="M45" s="29">
         <v>43</v>
       </c>
-      <c r="N45" s="32" t="s">
+      <c r="N45" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="O45" s="36" t="s">
+      <c r="O45" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P45" s="33" t="s">
+      <c r="P45" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3194,16 +3225,16 @@
       <c r="K46" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="M46" s="30">
+      <c r="M46" s="29">
         <v>44</v>
       </c>
-      <c r="N46" s="32" t="s">
+      <c r="N46" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="O46" s="36" t="s">
+      <c r="O46" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P46" s="33" t="s">
+      <c r="P46" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3221,22 +3252,22 @@
         <v>11</v>
       </c>
       <c r="G47" s="3"/>
-      <c r="H47" s="29">
+      <c r="H47" s="49">
         <v>42159</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="1"/>
       <c r="K47" s="12"/>
-      <c r="M47" s="30">
+      <c r="M47" s="29">
         <v>45</v>
       </c>
-      <c r="N47" s="32" t="s">
+      <c r="N47" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="O47" s="34" t="s">
+      <c r="O47" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P47" s="33" t="s">
+      <c r="P47" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3254,22 +3285,22 @@
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="29">
+      <c r="H48" s="49">
         <v>42159</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="1"/>
       <c r="K48" s="12"/>
-      <c r="M48" s="30">
+      <c r="M48" s="29">
         <v>46</v>
       </c>
-      <c r="N48" s="32" t="s">
+      <c r="N48" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="O48" s="34" t="s">
+      <c r="O48" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P48" s="33" t="s">
+      <c r="P48" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3287,22 +3318,22 @@
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="29">
+      <c r="H49" s="49">
         <v>42159</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="1"/>
       <c r="K49" s="12"/>
-      <c r="M49" s="30">
+      <c r="M49" s="29">
         <v>47</v>
       </c>
-      <c r="N49" s="32" t="s">
+      <c r="N49" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="O49" s="37" t="s">
+      <c r="O49" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P49" s="33" t="s">
+      <c r="P49" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3320,22 +3351,22 @@
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="29">
+      <c r="H50" s="49">
         <v>42159</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="1"/>
       <c r="K50" s="12"/>
-      <c r="M50" s="30">
+      <c r="M50" s="29">
         <v>48</v>
       </c>
-      <c r="N50" s="32" t="s">
+      <c r="N50" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="O50" s="37" t="s">
+      <c r="O50" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="P50" s="33" t="s">
+      <c r="P50" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3353,22 +3384,22 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
-      <c r="H51" s="29">
+      <c r="H51" s="49">
         <v>42159</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="1"/>
       <c r="K51" s="12"/>
-      <c r="M51" s="30">
+      <c r="M51" s="29">
         <v>49</v>
       </c>
-      <c r="N51" s="32" t="s">
+      <c r="N51" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="O51" s="36" t="s">
+      <c r="O51" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="P51" s="33" t="s">
+      <c r="P51" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3386,14 +3417,14 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="29">
+      <c r="H52" s="49">
         <v>42159</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="1"/>
       <c r="K52" s="12"/>
-      <c r="M52" s="38"/>
-      <c r="N52" s="39"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="38"/>
       <c r="P52"/>
       <c r="Q52"/>
     </row>
@@ -3411,14 +3442,14 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="29">
+      <c r="H53" s="49">
         <v>42159</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="1"/>
       <c r="K53" s="12"/>
-      <c r="M53" s="38"/>
-      <c r="N53" s="39"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="38"/>
       <c r="P53"/>
       <c r="Q53"/>
     </row>
@@ -3436,14 +3467,14 @@
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="29">
+      <c r="H54" s="49">
         <v>42159</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="1"/>
       <c r="K54" s="12"/>
-      <c r="M54" s="38"/>
-      <c r="N54" s="39"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="38"/>
       <c r="P54"/>
       <c r="Q54"/>
     </row>
@@ -3461,14 +3492,14 @@
       <c r="G55" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H55" s="29">
+      <c r="H55" s="49">
         <v>42159</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="1"/>
       <c r="K55" s="12"/>
-      <c r="M55" s="38"/>
-      <c r="N55" s="39"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="38"/>
       <c r="P55"/>
       <c r="Q55"/>
     </row>
@@ -3486,14 +3517,14 @@
       <c r="G56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H56" s="29">
+      <c r="H56" s="49">
         <v>42159</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="1"/>
       <c r="K56" s="12"/>
-      <c r="M56" s="38"/>
-      <c r="N56" s="39"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="38"/>
       <c r="P56"/>
       <c r="Q56"/>
     </row>
@@ -3511,14 +3542,14 @@
       <c r="G57" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H57" s="29">
+      <c r="H57" s="49">
         <v>42159</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="1"/>
       <c r="K57" s="12"/>
-      <c r="M57" s="38"/>
-      <c r="N57" s="39"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="38"/>
       <c r="P57"/>
       <c r="Q57"/>
     </row>
@@ -3536,14 +3567,14 @@
       <c r="G58" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="29">
+      <c r="H58" s="49">
         <v>42159</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="1"/>
       <c r="K58" s="12"/>
-      <c r="M58" s="38"/>
-      <c r="N58" s="39"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="38"/>
       <c r="P58"/>
       <c r="Q58"/>
     </row>
@@ -3561,14 +3592,14 @@
         <v>11</v>
       </c>
       <c r="G59" s="3"/>
-      <c r="H59" s="29">
+      <c r="H59" s="49">
         <v>42159</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="1"/>
       <c r="K59" s="12"/>
-      <c r="M59" s="38"/>
-      <c r="N59" s="39"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="38"/>
       <c r="P59"/>
       <c r="Q59"/>
     </row>
@@ -3577,17 +3608,25 @@
         <v>58</v>
       </c>
       <c r="B60" s="3"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
+      <c r="C60" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="48" t="s">
+        <v>11</v>
+      </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
+      <c r="H60" s="49">
+        <v>42160</v>
+      </c>
       <c r="I60" s="3"/>
       <c r="J60" s="1"/>
       <c r="K60" s="12"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="39"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="38"/>
       <c r="P60"/>
       <c r="Q60"/>
     </row>
@@ -3596,17 +3635,25 @@
         <v>59</v>
       </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
+      <c r="C61" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="48" t="s">
+        <v>11</v>
+      </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
+      <c r="H61" s="49">
+        <v>42160</v>
+      </c>
       <c r="I61" s="3"/>
       <c r="J61" s="1"/>
       <c r="K61" s="12"/>
-      <c r="M61" s="38"/>
-      <c r="N61" s="39"/>
+      <c r="M61" s="37"/>
+      <c r="N61" s="38"/>
       <c r="P61"/>
       <c r="Q61"/>
     </row>
@@ -3615,17 +3662,23 @@
         <v>58</v>
       </c>
       <c r="B62" s="3"/>
-      <c r="C62" s="4"/>
+      <c r="C62" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
+      <c r="G62" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" s="49">
+        <v>42160</v>
+      </c>
       <c r="I62" s="3"/>
       <c r="J62" s="1"/>
       <c r="K62" s="12"/>
-      <c r="M62" s="38"/>
-      <c r="N62" s="39"/>
+      <c r="M62" s="37"/>
+      <c r="N62" s="38"/>
       <c r="P62"/>
       <c r="Q62"/>
     </row>
@@ -3643,8 +3696,8 @@
       <c r="I63" s="3"/>
       <c r="J63" s="1"/>
       <c r="K63" s="12"/>
-      <c r="M63" s="38"/>
-      <c r="N63" s="39"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="38"/>
       <c r="P63"/>
       <c r="Q63"/>
     </row>
@@ -3662,8 +3715,8 @@
       <c r="I64" s="3"/>
       <c r="J64" s="1"/>
       <c r="K64" s="12"/>
-      <c r="M64" s="38"/>
-      <c r="N64" s="39"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="38"/>
       <c r="P64"/>
       <c r="Q64"/>
     </row>
@@ -3681,8 +3734,8 @@
       <c r="I65" s="3"/>
       <c r="J65" s="1"/>
       <c r="K65" s="12"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="39"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="38"/>
       <c r="P65"/>
       <c r="Q65"/>
     </row>
@@ -3700,8 +3753,8 @@
       <c r="I66" s="3"/>
       <c r="J66" s="1"/>
       <c r="K66" s="12"/>
-      <c r="M66" s="38"/>
-      <c r="N66" s="39"/>
+      <c r="M66" s="37"/>
+      <c r="N66" s="38"/>
       <c r="P66"/>
       <c r="Q66"/>
     </row>
@@ -3719,8 +3772,8 @@
       <c r="I67" s="3"/>
       <c r="J67" s="1"/>
       <c r="K67" s="12"/>
-      <c r="M67" s="38"/>
-      <c r="N67" s="39"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="38"/>
       <c r="P67"/>
       <c r="Q67"/>
     </row>
@@ -3738,8 +3791,8 @@
       <c r="I68" s="3"/>
       <c r="J68" s="1"/>
       <c r="K68" s="12"/>
-      <c r="M68" s="38"/>
-      <c r="N68" s="39"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="38"/>
       <c r="P68"/>
       <c r="Q68"/>
     </row>
@@ -3757,8 +3810,8 @@
       <c r="I69" s="3"/>
       <c r="J69" s="1"/>
       <c r="K69" s="12"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="39"/>
+      <c r="M69" s="37"/>
+      <c r="N69" s="38"/>
       <c r="P69"/>
       <c r="Q69"/>
     </row>
@@ -3776,8 +3829,8 @@
       <c r="I70" s="3"/>
       <c r="J70" s="1"/>
       <c r="K70" s="12"/>
-      <c r="M70" s="38"/>
-      <c r="N70" s="39"/>
+      <c r="M70" s="37"/>
+      <c r="N70" s="38"/>
       <c r="P70"/>
       <c r="Q70"/>
     </row>
@@ -3795,8 +3848,8 @@
       <c r="I71" s="3"/>
       <c r="J71" s="1"/>
       <c r="K71" s="12"/>
-      <c r="M71" s="38"/>
-      <c r="N71" s="39"/>
+      <c r="M71" s="37"/>
+      <c r="N71" s="38"/>
       <c r="P71"/>
       <c r="Q71"/>
     </row>
@@ -3814,8 +3867,8 @@
       <c r="I72" s="3"/>
       <c r="J72" s="1"/>
       <c r="K72" s="12"/>
-      <c r="M72" s="38"/>
-      <c r="N72" s="39"/>
+      <c r="M72" s="37"/>
+      <c r="N72" s="38"/>
       <c r="P72"/>
       <c r="Q72"/>
     </row>
@@ -3833,8 +3886,8 @@
       <c r="I73" s="3"/>
       <c r="J73" s="1"/>
       <c r="K73" s="12"/>
-      <c r="M73" s="38"/>
-      <c r="N73" s="39"/>
+      <c r="M73" s="37"/>
+      <c r="N73" s="38"/>
       <c r="P73"/>
       <c r="Q73"/>
     </row>
@@ -3852,8 +3905,8 @@
       <c r="I74" s="3"/>
       <c r="J74" s="1"/>
       <c r="K74" s="12"/>
-      <c r="M74" s="38"/>
-      <c r="N74" s="39"/>
+      <c r="M74" s="37"/>
+      <c r="N74" s="38"/>
       <c r="P74"/>
       <c r="Q74"/>
     </row>
@@ -3871,8 +3924,8 @@
       <c r="I75" s="3"/>
       <c r="J75" s="1"/>
       <c r="K75" s="12"/>
-      <c r="M75" s="38"/>
-      <c r="N75" s="39"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="38"/>
       <c r="P75"/>
       <c r="Q75"/>
     </row>
@@ -3890,8 +3943,8 @@
       <c r="I76" s="3"/>
       <c r="J76" s="1"/>
       <c r="K76" s="12"/>
-      <c r="M76" s="38"/>
-      <c r="N76" s="39"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="38"/>
       <c r="P76"/>
       <c r="Q76"/>
     </row>
@@ -3909,8 +3962,8 @@
       <c r="I77" s="3"/>
       <c r="J77" s="1"/>
       <c r="K77" s="12"/>
-      <c r="M77" s="38"/>
-      <c r="N77" s="39"/>
+      <c r="M77" s="37"/>
+      <c r="N77" s="38"/>
       <c r="P77"/>
       <c r="Q77"/>
     </row>
@@ -3928,8 +3981,8 @@
       <c r="I78" s="3"/>
       <c r="J78" s="1"/>
       <c r="K78" s="12"/>
-      <c r="M78" s="38"/>
-      <c r="N78" s="39"/>
+      <c r="M78" s="37"/>
+      <c r="N78" s="38"/>
       <c r="P78"/>
       <c r="Q78"/>
     </row>
@@ -3947,8 +4000,8 @@
       <c r="I79" s="3"/>
       <c r="J79" s="1"/>
       <c r="K79" s="12"/>
-      <c r="M79" s="38"/>
-      <c r="N79" s="39"/>
+      <c r="M79" s="37"/>
+      <c r="N79" s="38"/>
       <c r="P79"/>
       <c r="Q79"/>
     </row>
@@ -3966,8 +4019,8 @@
       <c r="I80" s="3"/>
       <c r="J80" s="1"/>
       <c r="K80" s="12"/>
-      <c r="M80" s="38"/>
-      <c r="N80" s="39"/>
+      <c r="M80" s="37"/>
+      <c r="N80" s="38"/>
       <c r="P80"/>
       <c r="Q80"/>
     </row>
@@ -3985,8 +4038,8 @@
       <c r="I81" s="3"/>
       <c r="J81" s="1"/>
       <c r="K81" s="12"/>
-      <c r="M81" s="38"/>
-      <c r="N81" s="39"/>
+      <c r="M81" s="37"/>
+      <c r="N81" s="38"/>
       <c r="P81"/>
       <c r="Q81"/>
     </row>
@@ -4004,8 +4057,8 @@
       <c r="I82" s="3"/>
       <c r="J82" s="1"/>
       <c r="K82" s="12"/>
-      <c r="M82" s="38"/>
-      <c r="N82" s="39"/>
+      <c r="M82" s="37"/>
+      <c r="N82" s="38"/>
       <c r="P82"/>
       <c r="Q82"/>
     </row>
@@ -4023,8 +4076,8 @@
       <c r="I83" s="3"/>
       <c r="J83" s="1"/>
       <c r="K83" s="12"/>
-      <c r="M83" s="38"/>
-      <c r="N83" s="39"/>
+      <c r="M83" s="37"/>
+      <c r="N83" s="38"/>
       <c r="P83"/>
       <c r="Q83"/>
     </row>
@@ -4042,8 +4095,8 @@
       <c r="I84" s="3"/>
       <c r="J84" s="1"/>
       <c r="K84" s="12"/>
-      <c r="M84" s="38"/>
-      <c r="N84" s="39"/>
+      <c r="M84" s="37"/>
+      <c r="N84" s="38"/>
       <c r="P84"/>
       <c r="Q84"/>
     </row>
@@ -4061,8 +4114,8 @@
       <c r="I85" s="3"/>
       <c r="J85" s="1"/>
       <c r="K85" s="12"/>
-      <c r="M85" s="38"/>
-      <c r="N85" s="39"/>
+      <c r="M85" s="37"/>
+      <c r="N85" s="38"/>
       <c r="P85"/>
       <c r="Q85"/>
     </row>
@@ -4080,8 +4133,8 @@
       <c r="I86" s="3"/>
       <c r="J86" s="1"/>
       <c r="K86" s="12"/>
-      <c r="M86" s="38"/>
-      <c r="N86" s="39"/>
+      <c r="M86" s="37"/>
+      <c r="N86" s="38"/>
       <c r="P86"/>
       <c r="Q86"/>
     </row>
@@ -4099,8 +4152,8 @@
       <c r="I87" s="3"/>
       <c r="J87" s="1"/>
       <c r="K87" s="12"/>
-      <c r="M87" s="38"/>
-      <c r="N87" s="39"/>
+      <c r="M87" s="37"/>
+      <c r="N87" s="38"/>
       <c r="P87"/>
       <c r="Q87"/>
     </row>
@@ -4118,8 +4171,8 @@
       <c r="I88" s="3"/>
       <c r="J88" s="1"/>
       <c r="K88" s="12"/>
-      <c r="M88" s="38"/>
-      <c r="N88" s="39"/>
+      <c r="M88" s="37"/>
+      <c r="N88" s="38"/>
       <c r="P88"/>
       <c r="Q88"/>
     </row>
@@ -4137,8 +4190,8 @@
       <c r="I89" s="3"/>
       <c r="J89" s="1"/>
       <c r="K89" s="12"/>
-      <c r="M89" s="38"/>
-      <c r="N89" s="39"/>
+      <c r="M89" s="37"/>
+      <c r="N89" s="38"/>
       <c r="P89"/>
       <c r="Q89"/>
     </row>
@@ -4156,8 +4209,8 @@
       <c r="I90" s="3"/>
       <c r="J90" s="1"/>
       <c r="K90" s="12"/>
-      <c r="M90" s="38"/>
-      <c r="N90" s="39"/>
+      <c r="M90" s="37"/>
+      <c r="N90" s="38"/>
       <c r="P90"/>
       <c r="Q90"/>
     </row>
@@ -4175,8 +4228,8 @@
       <c r="I91" s="3"/>
       <c r="J91" s="1"/>
       <c r="K91" s="12"/>
-      <c r="M91" s="38"/>
-      <c r="N91" s="39"/>
+      <c r="M91" s="37"/>
+      <c r="N91" s="38"/>
       <c r="P91"/>
       <c r="Q91"/>
     </row>
@@ -4194,8 +4247,8 @@
       <c r="I92" s="3"/>
       <c r="J92" s="1"/>
       <c r="K92" s="12"/>
-      <c r="M92" s="38"/>
-      <c r="N92" s="39"/>
+      <c r="M92" s="37"/>
+      <c r="N92" s="38"/>
       <c r="P92"/>
       <c r="Q92"/>
     </row>

</xml_diff>

<commit_message>
update 3 page lien quan toi assessment (NEED REVIEWER)
</commit_message>
<xml_diff>
--- a/Documents/Task Sheet/TaskSheet.xlsx
+++ b/Documents/Task Sheet/TaskSheet.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="420" windowWidth="13395" windowHeight="3615"/>
+    <workbookView xWindow="360" yWindow="480" windowWidth="13395" windowHeight="3555"/>
   </bookViews>
   <sheets>
-    <sheet name="150525-150526" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tasks Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Task Flow" sheetId="2" r:id="rId2"/>
+    <sheet name="Assess Info" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="204">
   <si>
     <t>No.</t>
   </si>
@@ -799,15 +799,6 @@
     <t>rp 2 va khung rp3(can ghi het cac khung use case)</t>
   </si>
   <si>
-    <t>html assessment for director</t>
-  </si>
-  <si>
-    <t>html assessment for staff</t>
-  </si>
-  <si>
-    <t>html assessment for manager</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -961,12 +952,60 @@
       <t>files</t>
     </r>
   </si>
+  <si>
+    <t>study send mail, random password string</t>
+  </si>
+  <si>
+    <t>1 man hinh co nut search va 1 drop down list chon assess period</t>
+  </si>
+  <si>
+    <t>initial load la assess moi nhat va dang cchay</t>
+  </si>
+  <si>
+    <t>director moi co quyen view het</t>
+  </si>
+  <si>
+    <t>role manager hay sstaff neu ko nam trong thoi ky danh gia thi ko dc view</t>
+  </si>
+  <si>
+    <t>direcctor la manager thi hien thi rra sao?</t>
+  </si>
+  <si>
+    <t>page 1: director assess manager(dung cho ca manager assess staff)</t>
+  </si>
+  <si>
+    <t>page 2: detail assess page</t>
+  </si>
+  <si>
+    <t>(dung chung cho ca 2 role manager va director view detail)</t>
+  </si>
+  <si>
+    <t>page 3: page hien assess do nguoi khac danh gia minh</t>
+  </si>
+  <si>
+    <t>assessmentPage</t>
+  </si>
+  <si>
+    <t>assessmentDetailPage</t>
+  </si>
+  <si>
+    <t>assessReceiversPage</t>
+  </si>
+  <si>
+    <t>html assessment Creator</t>
+  </si>
+  <si>
+    <t>html assessment Details</t>
+  </si>
+  <si>
+    <t>html assessment Receivers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,6 +1062,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
@@ -1133,10 +1181,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1269,8 +1318,13 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1574,7 +1628,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
+      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1631,7 +1685,7 @@
       </c>
       <c r="O1" s="44"/>
       <c r="P1" s="39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1667,10 +1721,10 @@
         <v>1</v>
       </c>
       <c r="O2" s="47" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1703,19 +1757,19 @@
         <v>1</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P3" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R3" s="41" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="S3" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1748,19 +1802,19 @@
         <v>2</v>
       </c>
       <c r="N4" s="31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P4" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R4" s="41" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S4" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1793,19 +1847,19 @@
         <v>3</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O5" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P5" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R5" s="41" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1834,19 +1888,19 @@
         <v>4</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O6" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P6" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R6" s="41" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="S6" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1875,13 +1929,13 @@
         <v>5</v>
       </c>
       <c r="N7" s="31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="O7" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P7" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="75">
@@ -1908,13 +1962,13 @@
         <v>6</v>
       </c>
       <c r="N8" s="31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P8" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -1943,13 +1997,13 @@
         <v>7</v>
       </c>
       <c r="N9" s="31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P9" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1978,13 +2032,13 @@
         <v>8</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="O10" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P10" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q10" s="40"/>
     </row>
@@ -2014,13 +2068,13 @@
         <v>9</v>
       </c>
       <c r="N11" s="31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P11" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -2049,13 +2103,13 @@
         <v>10</v>
       </c>
       <c r="N12" s="31" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O12" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P12" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -2080,13 +2134,13 @@
         <v>11</v>
       </c>
       <c r="N13" s="31" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="O13" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P13" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2117,13 +2171,13 @@
         <v>12</v>
       </c>
       <c r="N14" s="31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="O14" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P14" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P14" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -2152,13 +2206,13 @@
         <v>13</v>
       </c>
       <c r="N15" s="31" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="O15" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P15" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P15" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -2187,13 +2241,13 @@
         <v>14</v>
       </c>
       <c r="N16" s="31" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O16" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P16" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P16" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="60">
@@ -2222,13 +2276,13 @@
         <v>15</v>
       </c>
       <c r="N17" s="31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O17" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P17" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="30">
@@ -2257,13 +2311,13 @@
         <v>16</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O18" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P18" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30">
@@ -2292,13 +2346,13 @@
         <v>17</v>
       </c>
       <c r="N19" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P19" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2325,13 +2379,13 @@
         <v>18</v>
       </c>
       <c r="N20" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O20" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P20" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2358,13 +2412,13 @@
         <v>19</v>
       </c>
       <c r="N21" s="31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O21" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P21" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -2389,13 +2443,13 @@
         <v>20</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="O22" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P22" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2420,13 +2474,13 @@
         <v>21</v>
       </c>
       <c r="N23" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O23" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P23" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -2453,13 +2507,13 @@
         <v>22</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="O24" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P24" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2488,13 +2542,13 @@
         <v>23</v>
       </c>
       <c r="N25" s="31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O25" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P25" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2525,13 +2579,13 @@
         <v>24</v>
       </c>
       <c r="N26" s="31" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O26" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P26" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="30">
@@ -2560,13 +2614,13 @@
         <v>25</v>
       </c>
       <c r="N27" s="31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O27" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P27" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -2593,13 +2647,13 @@
         <v>26</v>
       </c>
       <c r="N28" s="31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O28" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P28" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P28" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="30">
@@ -2634,16 +2688,16 @@
         <v>27</v>
       </c>
       <c r="N29" s="31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="O29" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P29" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="P29" s="32" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="30">
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2675,13 +2729,13 @@
         <v>28</v>
       </c>
       <c r="N30" s="31" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O30" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P30" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P30" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2710,13 +2764,13 @@
         <v>29</v>
       </c>
       <c r="N31" s="31" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O31" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P31" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2745,13 +2799,13 @@
         <v>30</v>
       </c>
       <c r="N32" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O32" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P32" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2780,13 +2834,13 @@
         <v>31</v>
       </c>
       <c r="N33" s="31" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="O33" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P33" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="30">
@@ -2816,10 +2870,10 @@
         <v>60</v>
       </c>
       <c r="O34" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P34" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="30">
@@ -2849,10 +2903,10 @@
         <v>61</v>
       </c>
       <c r="O35" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P35" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="45">
@@ -2884,10 +2938,10 @@
         <v>62</v>
       </c>
       <c r="O36" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P36" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="90">
@@ -2917,10 +2971,10 @@
         <v>63</v>
       </c>
       <c r="O37" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P37" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P37" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -2950,10 +3004,10 @@
         <v>64</v>
       </c>
       <c r="O38" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P38" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P38" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -2983,10 +3037,10 @@
         <v>65</v>
       </c>
       <c r="O39" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P39" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P39" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="90">
@@ -3016,10 +3070,10 @@
         <v>66</v>
       </c>
       <c r="O40" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P40" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="30">
@@ -3046,13 +3100,13 @@
         <v>39</v>
       </c>
       <c r="N41" s="31" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="O41" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P41" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="30">
@@ -3081,13 +3135,13 @@
         <v>40</v>
       </c>
       <c r="N42" s="31" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O42" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P42" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3118,13 +3172,13 @@
         <v>41</v>
       </c>
       <c r="N43" s="31" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="O43" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P43" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3155,13 +3209,13 @@
         <v>42</v>
       </c>
       <c r="N44" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="O44" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P44" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="45">
@@ -3195,10 +3249,10 @@
         <v>67</v>
       </c>
       <c r="O45" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P45" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P45" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="45">
@@ -3232,10 +3286,10 @@
         <v>68</v>
       </c>
       <c r="O46" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P46" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P46" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3265,10 +3319,10 @@
         <v>70</v>
       </c>
       <c r="O47" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P47" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -3298,10 +3352,10 @@
         <v>75</v>
       </c>
       <c r="O48" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P48" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -3331,10 +3385,10 @@
         <v>69</v>
       </c>
       <c r="O49" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P49" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -3364,10 +3418,10 @@
         <v>76</v>
       </c>
       <c r="O50" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P50" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="30">
@@ -3375,10 +3429,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="3"/>
-      <c r="C51" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D51" s="3" t="s">
+      <c r="C51" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="3"/>
@@ -3394,13 +3448,13 @@
         <v>49</v>
       </c>
       <c r="N51" s="31" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="O51" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="P51" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="P51" s="32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -3408,10 +3462,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="3"/>
-      <c r="C52" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="C52" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="3"/>
@@ -3433,10 +3487,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="3"/>
-      <c r="C53" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D53" s="3" t="s">
+      <c r="C53" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="D53" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="3"/>
@@ -3609,7 +3663,7 @@
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D60" s="48" t="s">
         <v>11</v>
@@ -3636,7 +3690,7 @@
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D61" s="48" t="s">
         <v>11</v>
@@ -3663,7 +3717,7 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -3687,12 +3741,16 @@
         <v>59</v>
       </c>
       <c r="B63" s="3"/>
-      <c r="C63" s="4"/>
+      <c r="C63" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
+      <c r="H63" s="49">
+        <v>42160</v>
+      </c>
       <c r="I63" s="3"/>
       <c r="J63" s="1"/>
       <c r="K63" s="12"/>
@@ -4802,6 +4860,10 @@
       <c r="G173" s="14"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C51" location="'Assess Info'!A1" display="html assessment Creator"/>
+    <hyperlink ref="C52:C53" location="'Assess Info'!A1" display="html assessment Details"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4811,7 +4873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -5775,12 +5837,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A6:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>